<commit_message>
Test Commit From master
</commit_message>
<xml_diff>
--- a/GitTutorial/DataFolder/GitTutorial.xlsx
+++ b/GitTutorial/DataFolder/GitTutorial.xlsx
@@ -16,12 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>TestOne</t>
   </si>
   <si>
     <t>TestTwo</t>
+  </si>
+  <si>
+    <t>TestSheetOneFromMaster</t>
   </si>
 </sst>
 </file>
@@ -353,13 +356,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -368,6 +374,11 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit from master two
</commit_message>
<xml_diff>
--- a/GitTutorial/DataFolder/GitTutorial.xlsx
+++ b/GitTutorial/DataFolder/GitTutorial.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>TestOne</t>
   </si>
@@ -25,6 +25,9 @@
   </si>
   <si>
     <t>TestSheetOneFromMaster</t>
+  </si>
+  <si>
+    <t>TestSheetTwoFromMaster</t>
   </si>
 </sst>
 </file>
@@ -356,10 +359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -379,6 +382,11 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>